<commit_message>
test code commit by Kevin
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/excel/HistoricalExcel.xlsx
+++ b/src/test/resources/testData/excel/HistoricalExcel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
   <si>
     <t>Flow Type</t>
   </si>
@@ -245,6 +245,42 @@
   </si>
   <si>
     <t>Invoice1669556</t>
+  </si>
+  <si>
+    <t>Invoice1802129</t>
+  </si>
+  <si>
+    <t>Invoice1499983</t>
+  </si>
+  <si>
+    <t>Neil2892</t>
+  </si>
+  <si>
+    <t>Candy07dw</t>
+  </si>
+  <si>
+    <t>Invoice1348400</t>
+  </si>
+  <si>
+    <t>Invoice1494112</t>
+  </si>
+  <si>
+    <t>Laura036q</t>
+  </si>
+  <si>
+    <t>Lucye7o4</t>
+  </si>
+  <si>
+    <t>Invoice1511691</t>
+  </si>
+  <si>
+    <t>Invoice1825842</t>
+  </si>
+  <si>
+    <t>Invoice1393659</t>
+  </si>
+  <si>
+    <t>Invoice1881222</t>
   </si>
 </sst>
 </file>
@@ -1345,19 +1381,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D2" s="11">
         <v>44782</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>21</v>
@@ -1449,19 +1485,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6">
         <v>44782</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>